<commit_message>
Modified BOM, Add PCB documentation
</commit_message>
<xml_diff>
--- a/PCB/BOM/BOM V2 Combined.xlsx
+++ b/PCB/BOM/BOM V2 Combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molyo\OneDrive\Desktop\MIL\TailGator\PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A0DA18-44F1-4D1F-9F07-C3185B285127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F39E10C-DC9F-43FA-878D-B25BEFFBD8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" xr2:uid="{82F19887-029A-43E3-95FC-C827992C4836}"/>
+    <workbookView xWindow="28665" yWindow="-135" windowWidth="38670" windowHeight="21150" tabRatio="628" xr2:uid="{82F19887-029A-43E3-95FC-C827992C4836}"/>
   </bookViews>
   <sheets>
     <sheet name="COMBINED PT2" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="467">
   <si>
     <t>Line #</t>
   </si>
@@ -1455,6 +1455,12 @@
   </si>
   <si>
     <t>PDB V2 C1, C2</t>
+  </si>
+  <si>
+    <t>Emergency Order Qty</t>
+  </si>
+  <si>
+    <t>STAT?</t>
   </si>
 </sst>
 </file>
@@ -1508,7 +1514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1616,12 +1622,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1641,17 +1656,110 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{8BED9F05-ECF7-499E-893C-F1C4A348FB85}"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="35">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
         <i/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1732,84 +1840,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD3D3D3"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2050,13 +2080,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2069,6 +2092,31 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -2085,8 +2133,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC506BC4-14F3-4987-8435-E33CABD850AF}" name="RAW" displayName="RAW" ref="A1:M78" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="30" tableBorderDxfId="31" totalsRowBorderDxfId="29">
-  <autoFilter ref="A1:M78" xr:uid="{CC506BC4-14F3-4987-8435-E33CABD850AF}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC506BC4-14F3-4987-8435-E33CABD850AF}" name="RAW" displayName="RAW" ref="A1:N78" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+  <autoFilter ref="A1:N78" xr:uid="{CC506BC4-14F3-4987-8435-E33CABD850AF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2100,23 +2148,25 @@
     <filterColumn colId="10" hiddenButton="1"/>
     <filterColumn colId="11" hiddenButton="1"/>
     <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{02E8199E-69C0-41C2-9E9E-114981E956AF}" name="Line #" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{1383464D-F274-4339-9D66-9CA07FD1A079}" name="Name" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{9A03F236-8CD6-43D4-A246-9B2E595F82B2}" name="Description" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{639481CC-DC3E-4E4C-81BC-CF346B1E5DA7}" name="Designator" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{4FFFB3D1-C65B-467D-A98A-6B98E1512E6D}" name="Project Designator" dataDxfId="24">
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{02E8199E-69C0-41C2-9E9E-114981E956AF}" name="Line #" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{1383464D-F274-4339-9D66-9CA07FD1A079}" name="Name" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{9A03F236-8CD6-43D4-A246-9B2E595F82B2}" name="Description" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{639481CC-DC3E-4E4C-81BC-CF346B1E5DA7}" name="Designator" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{4FFFB3D1-C65B-467D-A98A-6B98E1512E6D}" name="Project Designator" dataDxfId="26">
       <calculatedColumnFormula>_xlfn.CONCAT("STAT V1 ", D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DCD9C2C1-D14C-44EB-9F00-943A0C0B0C86}" name="Quantity" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{D5538760-1111-4C44-85D2-972A60896936}" name="Supplier Order Qty 1" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{D14C02A3-E870-41DC-A6C4-D71AE1FD8C70}" name="Manufacturer" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{CAD794EC-800A-4A26-ABFE-1E0F2BD856B1}" name="Manufacturer  Part Number" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{C63698FA-B33F-44DD-A444-CEB0B8B9B4BA}" name="Supplier" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{7D6D4799-0C43-414A-9321-5C538DBDEFCF}" name="Supplier Part Number" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{9ADE6147-A2FA-43D4-BD36-12B72FDD0F3B}" name="Supplier Unit Price" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{BD929692-F2C5-4835-A717-564A8E0AA6E9}" name="Supplier Subtotal" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{DCD9C2C1-D14C-44EB-9F00-943A0C0B0C86}" name="Quantity" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{D5538760-1111-4C44-85D2-972A60896936}" name="Supplier Order Qty 1" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{9E40EE46-502F-4BD7-8280-D6439ABC74BD}" name="Emergency Order Qty" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{D14C02A3-E870-41DC-A6C4-D71AE1FD8C70}" name="Manufacturer" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{CAD794EC-800A-4A26-ABFE-1E0F2BD856B1}" name="Manufacturer  Part Number" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{C63698FA-B33F-44DD-A444-CEB0B8B9B4BA}" name="Supplier" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{7D6D4799-0C43-414A-9321-5C538DBDEFCF}" name="Supplier Part Number" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{9ADE6147-A2FA-43D4-BD36-12B72FDD0F3B}" name="Supplier Unit Price" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{BD929692-F2C5-4835-A717-564A8E0AA6E9}" name="Supplier Subtotal" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2439,18 +2489,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6A2F86-4998-4810-B01C-C1330CBD083D}">
-  <dimension ref="A1:I46"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="150.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="98.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="159.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.33203125" bestFit="1" customWidth="1"/>
@@ -2461,7 +2515,7 @@
     <col min="15" max="16" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2489,8 +2543,11 @@
       <c r="I1" s="6" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" s="19" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2509,8 +2566,8 @@
         <v>33</v>
       </c>
       <c r="F2" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H2)</f>
-        <v>90</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H2)</f>
+        <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -2521,8 +2578,12 @@
       <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" t="str">
+        <f>IF(ISNUMBER(SEARCH("STAT",D2)),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -2541,8 +2602,8 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H3)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H3)</f>
+        <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>65</v>
@@ -2553,8 +2614,12 @@
       <c r="I3" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K46" si="0">IF(ISNUMBER(SEARCH("STAT",D3)),"YES","NO")</f>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -2573,8 +2638,8 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H4)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H4)</f>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>65</v>
@@ -2585,8 +2650,12 @@
       <c r="I4" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -2605,8 +2674,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H5)</f>
-        <v>10</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H5)</f>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>76</v>
@@ -2617,8 +2686,12 @@
       <c r="I5" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -2637,8 +2710,8 @@
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H6)</f>
-        <v>8</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H6)</f>
+        <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>76</v>
@@ -2649,8 +2722,12 @@
       <c r="I6" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
@@ -2669,8 +2746,8 @@
         <v>4</v>
       </c>
       <c r="F7" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H7)</f>
-        <v>10</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H7)</f>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
@@ -2681,8 +2758,12 @@
       <c r="I7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -2701,8 +2782,8 @@
         <v>1</v>
       </c>
       <c r="F8" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H8)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H8)</f>
+        <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>30</v>
@@ -2713,8 +2794,12 @@
       <c r="I8" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>50</v>
       </c>
@@ -2733,8 +2818,8 @@
         <v>2</v>
       </c>
       <c r="F9" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H9)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H9)</f>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>98</v>
@@ -2745,8 +2830,12 @@
       <c r="I9" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -2765,8 +2854,8 @@
         <v>2</v>
       </c>
       <c r="F10" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H10)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H10)</f>
+        <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>104</v>
@@ -2777,8 +2866,12 @@
       <c r="I10" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>95</v>
       </c>
@@ -2797,8 +2890,8 @@
         <v>2</v>
       </c>
       <c r="F11" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H11)</f>
-        <v>10</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H11)</f>
+        <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
@@ -2809,8 +2902,12 @@
       <c r="I11" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>100</v>
       </c>
@@ -2829,8 +2926,8 @@
         <v>21</v>
       </c>
       <c r="F12" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H12)</f>
-        <v>60</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H12)</f>
+        <v>27</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>11</v>
@@ -2841,8 +2938,12 @@
       <c r="I12" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>106</v>
       </c>
@@ -2861,8 +2962,8 @@
         <v>2</v>
       </c>
       <c r="F13" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H13)</f>
-        <v>10</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H13)</f>
+        <v>4</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>11</v>
@@ -2873,8 +2974,12 @@
       <c r="I13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>111</v>
       </c>
@@ -2893,8 +2998,8 @@
         <v>3</v>
       </c>
       <c r="F14" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H14)</f>
-        <v>8</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H14)</f>
+        <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>30</v>
@@ -2905,8 +3010,12 @@
       <c r="I14" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>149</v>
       </c>
@@ -2925,8 +3034,8 @@
         <v>4</v>
       </c>
       <c r="F15" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H15)</f>
-        <v>16</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H15)</f>
+        <v>8</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>36</v>
@@ -2937,8 +3046,12 @@
       <c r="I15" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>231</v>
       </c>
@@ -2957,8 +3070,8 @@
         <v>4</v>
       </c>
       <c r="F16" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H16)</f>
-        <v>16</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H16)</f>
+        <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>11</v>
@@ -2969,8 +3082,12 @@
       <c r="I16" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>153</v>
       </c>
@@ -2989,8 +3106,8 @@
         <v>4</v>
       </c>
       <c r="F17" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H17)</f>
-        <v>16</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H17)</f>
+        <v>8</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>11</v>
@@ -3001,8 +3118,12 @@
       <c r="I17" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>155</v>
       </c>
@@ -3021,8 +3142,8 @@
         <v>2</v>
       </c>
       <c r="F18" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H18)</f>
-        <v>8</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H18)</f>
+        <v>4</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>59</v>
@@ -3033,8 +3154,12 @@
       <c r="I18" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>246</v>
       </c>
@@ -3053,8 +3178,8 @@
         <v>1</v>
       </c>
       <c r="F19" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H19)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H19)</f>
+        <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>142</v>
@@ -3065,8 +3190,12 @@
       <c r="I19" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>160</v>
       </c>
@@ -3085,8 +3214,8 @@
         <v>1</v>
       </c>
       <c r="F20" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H20)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H20)</f>
+        <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>218</v>
@@ -3097,8 +3226,12 @@
       <c r="I20" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>165</v>
       </c>
@@ -3117,7 +3250,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H21)</f>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H21)</f>
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -3129,8 +3262,12 @@
       <c r="I21" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>172</v>
       </c>
@@ -3149,8 +3286,8 @@
         <v>1</v>
       </c>
       <c r="F22" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H22)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H22)</f>
+        <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>36</v>
@@ -3161,8 +3298,12 @@
       <c r="I22" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>177</v>
       </c>
@@ -3181,8 +3322,8 @@
         <v>1</v>
       </c>
       <c r="F23" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H23)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H23)</f>
+        <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>36</v>
@@ -3193,8 +3334,12 @@
       <c r="I23" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>184</v>
       </c>
@@ -3213,8 +3358,8 @@
         <v>1</v>
       </c>
       <c r="F24" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H24)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H24)</f>
+        <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>65</v>
@@ -3225,8 +3370,12 @@
       <c r="I24" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>191</v>
       </c>
@@ -3245,8 +3394,8 @@
         <v>1</v>
       </c>
       <c r="F25" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H25)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H25)</f>
+        <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>244</v>
@@ -3257,8 +3406,12 @@
       <c r="I25" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>198</v>
       </c>
@@ -3277,8 +3430,8 @@
         <v>2</v>
       </c>
       <c r="F26" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H26)</f>
-        <v>10</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H26)</f>
+        <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>11</v>
@@ -3289,8 +3442,12 @@
       <c r="I26" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>204</v>
       </c>
@@ -3309,8 +3466,8 @@
         <v>2</v>
       </c>
       <c r="F27" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H27)</f>
-        <v>10</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H27)</f>
+        <v>2</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>257</v>
@@ -3321,8 +3478,12 @@
       <c r="I27" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>260</v>
       </c>
@@ -3341,8 +3502,8 @@
         <v>1</v>
       </c>
       <c r="F28" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H28)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H28)</f>
+        <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>267</v>
@@ -3353,8 +3514,12 @@
       <c r="I28" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>261</v>
       </c>
@@ -3373,8 +3538,8 @@
         <v>1</v>
       </c>
       <c r="F29" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H29)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H29)</f>
+        <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>65</v>
@@ -3385,8 +3550,12 @@
       <c r="I29" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>262</v>
       </c>
@@ -3405,8 +3574,8 @@
         <v>1</v>
       </c>
       <c r="F30" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H30)</f>
-        <v>2</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H30)</f>
+        <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>281</v>
@@ -3417,8 +3586,12 @@
       <c r="I30" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>263</v>
       </c>
@@ -3437,8 +3610,8 @@
         <v>8</v>
       </c>
       <c r="F31" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H31)</f>
-        <v>20</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H31)</f>
+        <v>8</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>11</v>
@@ -3449,8 +3622,12 @@
       <c r="I31" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>264</v>
       </c>
@@ -3469,8 +3646,8 @@
         <v>4</v>
       </c>
       <c r="F32" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H32)</f>
-        <v>20</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H32)</f>
+        <v>4</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>11</v>
@@ -3481,8 +3658,12 @@
       <c r="I32" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>270</v>
       </c>
@@ -3501,8 +3682,8 @@
         <v>2</v>
       </c>
       <c r="F33" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H33)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H33)</f>
+        <v>2</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>76</v>
@@ -3513,8 +3694,12 @@
       <c r="I33" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K33" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>275</v>
       </c>
@@ -3533,8 +3718,8 @@
         <v>2</v>
       </c>
       <c r="F34" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H34)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H34)</f>
+        <v>2</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>131</v>
@@ -3545,8 +3730,12 @@
       <c r="I34" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K34" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>277</v>
       </c>
@@ -3565,8 +3754,8 @@
         <v>2</v>
       </c>
       <c r="F35" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H35)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H35)</f>
+        <v>2</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>136</v>
@@ -3577,8 +3766,12 @@
       <c r="I35" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K35" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>283</v>
       </c>
@@ -3597,8 +3790,8 @@
         <v>4</v>
       </c>
       <c r="F36" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H36)</f>
-        <v>8</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H36)</f>
+        <v>4</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>147</v>
@@ -3609,8 +3802,12 @@
       <c r="I36" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K36" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>325</v>
       </c>
@@ -3629,8 +3826,8 @@
         <v>4</v>
       </c>
       <c r="F37" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H37)</f>
-        <v>20</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H37)</f>
+        <v>4</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>11</v>
@@ -3641,8 +3838,12 @@
       <c r="I37" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K37" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>326</v>
       </c>
@@ -3661,8 +3862,8 @@
         <v>4</v>
       </c>
       <c r="F38" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H38)</f>
-        <v>20</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H38)</f>
+        <v>4</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>11</v>
@@ -3673,8 +3874,12 @@
       <c r="I38" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K38" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>327</v>
       </c>
@@ -3693,8 +3898,8 @@
         <v>5</v>
       </c>
       <c r="F39" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H39)</f>
-        <v>20</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H39)</f>
+        <v>5</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>11</v>
@@ -3705,8 +3910,12 @@
       <c r="I39" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K39" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>328</v>
       </c>
@@ -3725,8 +3934,8 @@
         <v>4</v>
       </c>
       <c r="F40" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H40)</f>
-        <v>8</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H40)</f>
+        <v>4</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>169</v>
@@ -3737,8 +3946,12 @@
       <c r="I40" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K40" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>329</v>
       </c>
@@ -3757,8 +3970,8 @@
         <v>2</v>
       </c>
       <c r="F41" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H41)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H41)</f>
+        <v>2</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>169</v>
@@ -3769,8 +3982,12 @@
       <c r="I41" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K41" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>330</v>
       </c>
@@ -3789,8 +4006,8 @@
         <v>2</v>
       </c>
       <c r="F42" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H42)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H42)</f>
+        <v>2</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>181</v>
@@ -3801,8 +4018,12 @@
       <c r="I42" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>331</v>
       </c>
@@ -3821,8 +4042,8 @@
         <v>2</v>
       </c>
       <c r="F43" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H43)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H43)</f>
+        <v>2</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>188</v>
@@ -3833,8 +4054,12 @@
       <c r="I43" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K43" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>332</v>
       </c>
@@ -3853,8 +4078,8 @@
         <v>2</v>
       </c>
       <c r="F44" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H44)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H44)</f>
+        <v>2</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>195</v>
@@ -3865,8 +4090,12 @@
       <c r="I44" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K44" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>333</v>
       </c>
@@ -3885,8 +4114,8 @@
         <v>2</v>
       </c>
       <c r="F45" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H45)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H45)</f>
+        <v>2</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>195</v>
@@ -3897,8 +4126,12 @@
       <c r="I45" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K45" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>334</v>
       </c>
@@ -3917,8 +4150,8 @@
         <v>2</v>
       </c>
       <c r="F46" s="2">
-        <f>SUMIFS(RAW[Supplier Order Qty 1],RAW[Manufacturer  Part Number],$H46)</f>
-        <v>4</v>
+        <f>SUMIFS(RAW[Emergency Order Qty],RAW[Manufacturer  Part Number],$H46)</f>
+        <v>2</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>208</v>
@@ -3929,49 +4162,64 @@
       <c r="I46" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="K46" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="H1:I1 K1">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:I11 H47:I1048576 K1">
+    <cfRule type="duplicateValues" dxfId="16" priority="12"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H2:I2">
+    <cfRule type="duplicateValues" dxfId="15" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:I4">
     <cfRule type="duplicateValues" dxfId="14" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1">
+  <conditionalFormatting sqref="H5:I5">
     <cfRule type="duplicateValues" dxfId="13" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I4">
+  <conditionalFormatting sqref="H6:I6">
     <cfRule type="duplicateValues" dxfId="12" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I5">
+  <conditionalFormatting sqref="H7:I7">
     <cfRule type="duplicateValues" dxfId="11" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:I6">
+  <conditionalFormatting sqref="H8:I11">
     <cfRule type="duplicateValues" dxfId="10" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:I7">
-    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8:I11">
-    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I11 H47:I1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H12:I12">
-    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:I13">
-    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:I14">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:I30">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31:I46">
-    <cfRule type="duplicateValues" dxfId="2" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="24"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",K1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="R3">
+      <formula>NOT(ISERROR(SEARCH("R3",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="72" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6461,15 +6709,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF691AD3-4FF5-442E-B194-F0F49B405A9C}">
-  <dimension ref="A1:M78"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView topLeftCell="D53" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:E78"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23:H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6481,15 +6730,16 @@
     <col min="5" max="5" width="66" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6512,25 +6762,28 @@
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -6553,26 +6806,30 @@
       <c r="G2" s="2">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>0.1</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -6595,26 +6852,30 @@
       <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>0.21</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>0.42</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -6637,26 +6898,30 @@
       <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>0.21</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>0.42</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -6679,26 +6944,30 @@
       <c r="G5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>0.15</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -6721,26 +6990,30 @@
       <c r="G6" s="2">
         <v>2</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>0.15</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
@@ -6763,26 +7036,30 @@
       <c r="G7" s="12">
         <v>4</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="L7" s="12">
+      <c r="M7" s="12">
         <v>0.98</v>
       </c>
-      <c r="M7" s="13">
+      <c r="N7" s="13">
         <v>3.92</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -6805,26 +7082,30 @@
       <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>1.72</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <v>3.44</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>50</v>
       </c>
@@ -6847,26 +7128,30 @@
       <c r="G9" s="2">
         <v>2</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>1.89</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>3.78</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
@@ -6889,26 +7174,30 @@
       <c r="G10" s="2">
         <v>4</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>0.31</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <v>1.24</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>95</v>
       </c>
@@ -6931,26 +7220,30 @@
       <c r="G11" s="2">
         <v>4</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>0.44</v>
       </c>
-      <c r="M11" s="4">
+      <c r="N11" s="4">
         <v>1.76</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>100</v>
       </c>
@@ -6973,26 +7266,30 @@
       <c r="G12" s="2">
         <v>10</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M12" s="4">
+      <c r="N12" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>106</v>
       </c>
@@ -7015,26 +7312,30 @@
       <c r="G13" s="2">
         <v>10</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>111</v>
       </c>
@@ -7057,26 +7358,30 @@
       <c r="G14" s="2">
         <v>10</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>4</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <v>0.42</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>149</v>
       </c>
@@ -7099,26 +7404,30 @@
       <c r="G15" s="2">
         <v>10</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>4</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="M15" s="4">
+      <c r="N15" s="4">
         <v>0.69</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>231</v>
       </c>
@@ -7141,26 +7450,30 @@
       <c r="G16" s="2">
         <v>4</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>1.72</v>
       </c>
-      <c r="M16" s="4">
+      <c r="N16" s="4">
         <v>6.88</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>153</v>
       </c>
@@ -7183,26 +7496,30 @@
       <c r="G17" s="2">
         <v>4</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>1.38</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <v>5.52</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>155</v>
       </c>
@@ -7225,26 +7542,30 @@
       <c r="G18" s="2">
         <v>16</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>8</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>0.315</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <v>5.04</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>246</v>
       </c>
@@ -7267,26 +7588,30 @@
       <c r="G19" s="2">
         <v>24</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>12</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L19" s="2">
+      <c r="M19" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M19" s="4">
+      <c r="N19" s="4">
         <v>0.45600000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>160</v>
       </c>
@@ -7309,26 +7634,30 @@
       <c r="G20" s="2">
         <v>16</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>8</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L20" s="2">
+      <c r="M20" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M20" s="4">
+      <c r="N20" s="4">
         <v>0.24</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>165</v>
       </c>
@@ -7351,26 +7680,30 @@
       <c r="G21" s="2">
         <v>16</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>8</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L21" s="2">
+      <c r="M21" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M21" s="4">
+      <c r="N21" s="4">
         <v>0.30399999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>172</v>
       </c>
@@ -7393,26 +7726,30 @@
       <c r="G22" s="2">
         <v>8</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="2">
+        <f>RAW[[#This Row],[Quantity]]*2</f>
+        <v>4</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L22" s="2">
+      <c r="M22" s="2">
         <v>1.53</v>
       </c>
-      <c r="M22" s="4">
+      <c r="N22" s="4">
         <v>12.24</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>177</v>
       </c>
@@ -7435,26 +7772,30 @@
       <c r="G23" s="2">
         <v>10</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>4</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="L23" s="2">
+      <c r="M23" s="2">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="M23" s="4">
+      <c r="N23" s="4">
         <v>0.66</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>184</v>
       </c>
@@ -7477,26 +7818,30 @@
       <c r="G24" s="2">
         <v>26</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>13</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L24" s="2">
+      <c r="M24" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="M24" s="4">
+      <c r="N24" s="4">
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>191</v>
       </c>
@@ -7519,26 +7864,30 @@
       <c r="G25" s="2">
         <v>10</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L25" s="2">
+      <c r="M25" s="2">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="M25" s="4">
+      <c r="N25" s="4">
         <v>0.33</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>198</v>
       </c>
@@ -7561,26 +7910,30 @@
       <c r="G26" s="2">
         <v>2</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L26" s="2">
+      <c r="M26" s="2">
         <v>0.15</v>
       </c>
-      <c r="M26" s="4">
+      <c r="N26" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>204</v>
       </c>
@@ -7603,26 +7956,30 @@
       <c r="G27" s="2">
         <v>4</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L27" s="2">
+      <c r="M27" s="2">
         <v>0.15</v>
       </c>
-      <c r="M27" s="4">
+      <c r="N27" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>260</v>
       </c>
@@ -7645,26 +8002,30 @@
       <c r="G28" s="2">
         <v>2</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L28" s="2">
+      <c r="M28" s="2">
         <v>1.72</v>
       </c>
-      <c r="M28" s="4">
+      <c r="N28" s="4">
         <v>3.44</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>261</v>
       </c>
@@ -7687,26 +8048,30 @@
       <c r="G29" s="2">
         <v>2</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L29" s="2">
+      <c r="M29" s="2">
         <v>1.38</v>
       </c>
-      <c r="M29" s="4">
+      <c r="N29" s="4">
         <v>2.76</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>262</v>
       </c>
@@ -7729,26 +8094,30 @@
       <c r="G30" s="2">
         <v>2</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="L30" s="2">
+      <c r="M30" s="2">
         <v>0.81</v>
       </c>
-      <c r="M30" s="4">
+      <c r="N30" s="4">
         <v>1.62</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>263</v>
       </c>
@@ -7771,26 +8140,30 @@
       <c r="G31" s="2">
         <v>2</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="L31" s="2">
+      <c r="M31" s="2">
         <v>0.76</v>
       </c>
-      <c r="M31" s="4">
+      <c r="N31" s="4">
         <v>1.52</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>264</v>
       </c>
@@ -7813,26 +8186,30 @@
       <c r="G32" s="2">
         <v>2</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="L32" s="2">
+      <c r="M32" s="2">
         <v>0.24</v>
       </c>
-      <c r="M32" s="4">
+      <c r="N32" s="4">
         <v>0.48</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>270</v>
       </c>
@@ -7855,26 +8232,30 @@
       <c r="G33" s="2">
         <v>2</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L33" s="2">
+      <c r="M33" s="2">
         <v>0.15</v>
       </c>
-      <c r="M33" s="4">
+      <c r="N33" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>275</v>
       </c>
@@ -7897,26 +8278,30 @@
       <c r="G34" s="2">
         <v>4</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="L34" s="2">
+      <c r="M34" s="2">
         <v>0.13</v>
       </c>
-      <c r="M34" s="4">
+      <c r="N34" s="4">
         <v>0.52</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>277</v>
       </c>
@@ -7939,26 +8324,30 @@
       <c r="G35" s="2">
         <v>10</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="L35" s="2">
+      <c r="M35" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M35" s="4">
+      <c r="N35" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>283</v>
       </c>
@@ -7981,26 +8370,30 @@
       <c r="G36" s="2">
         <v>10</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H36" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>5</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L36" s="2">
+      <c r="M36" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M36" s="4">
+      <c r="N36" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>325</v>
       </c>
@@ -8023,26 +8416,30 @@
       <c r="G37" s="2">
         <v>10</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H37" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L37" s="2">
+      <c r="M37" s="2">
         <v>0.02</v>
       </c>
-      <c r="M37" s="4">
+      <c r="N37" s="4">
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>326</v>
       </c>
@@ -8065,26 +8462,30 @@
       <c r="G38" s="2">
         <v>10</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L38" s="2">
+      <c r="M38" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M38" s="4">
+      <c r="N38" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>327</v>
       </c>
@@ -8107,26 +8508,30 @@
       <c r="G39" s="2">
         <v>4</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L39" s="2">
+      <c r="M39" s="2">
         <v>0.34</v>
       </c>
-      <c r="M39" s="4">
+      <c r="N39" s="4">
         <v>1.36</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>328</v>
       </c>
@@ -8149,26 +8554,30 @@
       <c r="G40" s="2">
         <v>2</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L40" s="2">
+      <c r="M40" s="2">
         <v>0.73</v>
       </c>
-      <c r="M40" s="4">
+      <c r="N40" s="4">
         <v>1.46</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>329</v>
       </c>
@@ -8191,26 +8600,30 @@
       <c r="G41" s="2">
         <v>2</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L41" s="2">
+      <c r="M41" s="2">
         <v>0.7</v>
       </c>
-      <c r="M41" s="4">
+      <c r="N41" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>330</v>
       </c>
@@ -8233,26 +8646,30 @@
       <c r="G42" s="2">
         <v>2</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L42" s="2">
+      <c r="M42" s="2">
         <v>1.78</v>
       </c>
-      <c r="M42" s="4">
+      <c r="N42" s="4">
         <v>3.56</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>331</v>
       </c>
@@ -8275,26 +8692,30 @@
       <c r="G43" s="2">
         <v>2</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="L43" s="2">
+      <c r="M43" s="2">
         <v>0.83</v>
       </c>
-      <c r="M43" s="4">
+      <c r="N43" s="4">
         <v>1.66</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>332</v>
       </c>
@@ -8317,26 +8738,30 @@
       <c r="G44" s="2">
         <v>2</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L44" s="2">
+      <c r="M44" s="2">
         <v>0.46</v>
       </c>
-      <c r="M44" s="4">
+      <c r="N44" s="4">
         <v>0.92</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>333</v>
       </c>
@@ -8359,26 +8784,30 @@
       <c r="G45" s="2">
         <v>2</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="K45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="L45" s="2">
+      <c r="M45" s="2">
         <v>0.24</v>
       </c>
-      <c r="M45" s="4">
+      <c r="N45" s="4">
         <v>0.48</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>334</v>
       </c>
@@ -8401,26 +8830,30 @@
       <c r="G46" s="2">
         <v>10</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>4</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="L46" s="2">
+      <c r="M46" s="2">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="M46" s="4">
+      <c r="N46" s="4">
         <v>0.66</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>335</v>
       </c>
@@ -8443,26 +8876,30 @@
       <c r="G47" s="2">
         <v>50</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>16</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L47" s="2">
+      <c r="M47" s="2">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="M47" s="4">
+      <c r="N47" s="4">
         <v>1.19</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>336</v>
       </c>
@@ -8485,26 +8922,30 @@
       <c r="G48" s="2">
         <v>10</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L48" s="2">
+      <c r="M48" s="2">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="M48" s="4">
+      <c r="N48" s="4">
         <v>0.33</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>337</v>
       </c>
@@ -8527,26 +8968,30 @@
       <c r="G49" s="2">
         <v>4</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H49" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L49" s="2">
+      <c r="M49" s="2">
         <v>0.15</v>
       </c>
-      <c r="M49" s="4">
+      <c r="N49" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>338</v>
       </c>
@@ -8569,26 +9014,30 @@
       <c r="G50" s="2">
         <v>2</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H50" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L50" s="2">
+      <c r="M50" s="2">
         <v>0.15</v>
       </c>
-      <c r="M50" s="4">
+      <c r="N50" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>339</v>
       </c>
@@ -8611,26 +9060,30 @@
       <c r="G51" s="2">
         <v>4</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H51" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L51" s="2">
+      <c r="M51" s="2">
         <v>0.15</v>
       </c>
-      <c r="M51" s="4">
+      <c r="N51" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>340</v>
       </c>
@@ -8653,26 +9106,30 @@
       <c r="G52" s="2">
         <v>2</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="H52" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="L52" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L52" s="2">
+      <c r="M52" s="2">
         <v>1.72</v>
       </c>
-      <c r="M52" s="4">
+      <c r="N52" s="4">
         <v>3.44</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>341</v>
       </c>
@@ -8695,26 +9152,30 @@
       <c r="G53" s="2">
         <v>2</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="H53" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="K53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="L53" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L53" s="2">
+      <c r="M53" s="2">
         <v>1.38</v>
       </c>
-      <c r="M53" s="4">
+      <c r="N53" s="4">
         <v>2.76</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>342</v>
       </c>
@@ -8737,26 +9198,30 @@
       <c r="G54" s="2">
         <v>2</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="J54" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="K54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="L54" s="2">
+      <c r="M54" s="2">
         <v>0.81</v>
       </c>
-      <c r="M54" s="4">
+      <c r="N54" s="4">
         <v>1.62</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>343</v>
       </c>
@@ -8779,26 +9244,30 @@
       <c r="G55" s="2">
         <v>2</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H55" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="L55" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="L55" s="2">
+      <c r="M55" s="2">
         <v>0.76</v>
       </c>
-      <c r="M55" s="4">
+      <c r="N55" s="4">
         <v>1.52</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>344</v>
       </c>
@@ -8821,26 +9290,30 @@
       <c r="G56" s="2">
         <v>2</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I56" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="J56" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="K56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="L56" s="2">
+      <c r="M56" s="2">
         <v>1.2</v>
       </c>
-      <c r="M56" s="4">
+      <c r="N56" s="4">
         <v>2.4</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>345</v>
       </c>
@@ -8863,26 +9336,30 @@
       <c r="G57" s="2">
         <v>1</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="H57" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="J57" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="K57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="L57" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="L57" s="2">
+      <c r="M57" s="2">
         <v>14.95</v>
       </c>
-      <c r="M57" s="4">
+      <c r="N57" s="4">
         <v>14.95</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>346</v>
       </c>
@@ -8905,26 +9382,30 @@
       <c r="G58" s="2">
         <v>2</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="H58" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I58" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="K58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="L58" s="2">
+      <c r="M58" s="2">
         <v>0.43</v>
       </c>
-      <c r="M58" s="4">
+      <c r="N58" s="4">
         <v>0.86</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>347</v>
       </c>
@@ -8947,26 +9428,30 @@
       <c r="G59" s="2">
         <v>2</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="H59" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="J59" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="K59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="L59" s="2">
+      <c r="M59" s="2">
         <v>0.64</v>
       </c>
-      <c r="M59" s="4">
+      <c r="N59" s="4">
         <v>1.28</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>348</v>
       </c>
@@ -8989,26 +9474,30 @@
       <c r="G60" s="2">
         <v>2</v>
       </c>
-      <c r="H60" s="1" t="s">
+      <c r="H60" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="L60" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="L60" s="2">
+      <c r="M60" s="2">
         <v>0.41</v>
       </c>
-      <c r="M60" s="4">
+      <c r="N60" s="4">
         <v>0.82</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>349</v>
       </c>
@@ -9031,26 +9520,30 @@
       <c r="G61" s="2">
         <v>2</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="H61" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="I61" s="1" t="s">
+      <c r="J61" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="J61" s="1" t="s">
+      <c r="K61" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="L61" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="L61" s="2">
+      <c r="M61" s="2">
         <v>0.43</v>
       </c>
-      <c r="M61" s="4">
+      <c r="N61" s="4">
         <v>0.86</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>350</v>
       </c>
@@ -9073,26 +9566,30 @@
       <c r="G62" s="2">
         <v>4</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="H62" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J62" s="1" t="s">
+      <c r="K62" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="L62" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L62" s="2">
+      <c r="M62" s="2">
         <v>0.11890000000000001</v>
       </c>
-      <c r="M62" s="4">
+      <c r="N62" s="4">
         <v>0.47560000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>351</v>
       </c>
@@ -9115,26 +9612,30 @@
       <c r="G63" s="2">
         <v>10</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="H63" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="1" t="s">
+      <c r="J63" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J63" s="1" t="s">
+      <c r="K63" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K63" s="1" t="s">
+      <c r="L63" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="L63" s="2">
+      <c r="M63" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M63" s="4">
+      <c r="N63" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>352</v>
       </c>
@@ -9157,26 +9658,30 @@
       <c r="G64" s="2">
         <v>16</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="H64" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>8</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I64" s="1" t="s">
+      <c r="J64" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J64" s="1" t="s">
+      <c r="K64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K64" s="1" t="s">
+      <c r="L64" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L64" s="2">
+      <c r="M64" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M64" s="4">
+      <c r="N64" s="4">
         <v>0.30399999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>353</v>
       </c>
@@ -9199,26 +9704,30 @@
       <c r="G65" s="2">
         <v>10</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="H65" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I65" s="1" t="s">
+      <c r="J65" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="J65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="L65" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="L65" s="2">
+      <c r="M65" s="2">
         <v>0.02</v>
       </c>
-      <c r="M65" s="4">
+      <c r="N65" s="4">
         <v>0.2</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>354</v>
       </c>
@@ -9241,26 +9750,30 @@
       <c r="G66" s="2">
         <v>10</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="H66" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="J66" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="K66" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="L66" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="L66" s="2">
+      <c r="M66" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M66" s="4">
+      <c r="N66" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>355</v>
       </c>
@@ -9283,26 +9796,30 @@
       <c r="G67" s="2">
         <v>10</v>
       </c>
-      <c r="H67" s="1" t="s">
+      <c r="H67" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>3</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I67" s="1" t="s">
+      <c r="J67" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J67" s="1" t="s">
+      <c r="K67" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K67" s="1" t="s">
+      <c r="L67" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L67" s="2">
+      <c r="M67" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="M67" s="4">
+      <c r="N67" s="4">
         <v>0.19</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>356</v>
       </c>
@@ -9325,26 +9842,30 @@
       <c r="G68" s="2">
         <v>10</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="H68" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I68" s="1" t="s">
+      <c r="J68" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="K68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K68" s="1" t="s">
+      <c r="L68" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="L68" s="2">
+      <c r="M68" s="2">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="M68" s="4">
+      <c r="N68" s="4">
         <v>0.21</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>357</v>
       </c>
@@ -9367,26 +9888,30 @@
       <c r="G69" s="2">
         <v>4</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="H69" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>2</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="J69" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="K69" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="L69" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L69" s="2">
+      <c r="M69" s="2">
         <v>0.34</v>
       </c>
-      <c r="M69" s="4">
+      <c r="N69" s="4">
         <v>1.36</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>358</v>
       </c>
@@ -9409,26 +9934,30 @@
       <c r="G70" s="2">
         <v>2</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H70" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I70" s="1" t="s">
+      <c r="J70" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J70" s="1" t="s">
+      <c r="K70" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="L70" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L70" s="2">
+      <c r="M70" s="2">
         <v>0.73</v>
       </c>
-      <c r="M70" s="4">
+      <c r="N70" s="4">
         <v>1.46</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>359</v>
       </c>
@@ -9451,26 +9980,30 @@
       <c r="G71" s="2">
         <v>2</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="H71" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I71" s="1" t="s">
+      <c r="J71" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J71" s="1" t="s">
+      <c r="K71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K71" s="1" t="s">
+      <c r="L71" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L71" s="2">
+      <c r="M71" s="2">
         <v>0.7</v>
       </c>
-      <c r="M71" s="4">
+      <c r="N71" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>360</v>
       </c>
@@ -9493,26 +10026,30 @@
       <c r="G72" s="2">
         <v>2</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="H72" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I72" s="1" t="s">
+      <c r="J72" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="J72" s="1" t="s">
+      <c r="K72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K72" s="1" t="s">
+      <c r="L72" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L72" s="2">
+      <c r="M72" s="2">
         <v>1.78</v>
       </c>
-      <c r="M72" s="4">
+      <c r="N72" s="4">
         <v>3.56</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>361</v>
       </c>
@@ -9535,26 +10072,30 @@
       <c r="G73" s="2">
         <v>2</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="H73" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I73" s="1" t="s">
+      <c r="J73" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="J73" s="1" t="s">
+      <c r="K73" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="L73" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L73" s="2">
+      <c r="M73" s="2">
         <v>0.46</v>
       </c>
-      <c r="M73" s="4">
+      <c r="N73" s="4">
         <v>0.92</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>362</v>
       </c>
@@ -9577,26 +10118,30 @@
       <c r="G74" s="2">
         <v>2</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="H74" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="J74" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="K74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="L74" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="L74" s="2">
+      <c r="M74" s="2">
         <v>1.77</v>
       </c>
-      <c r="M74" s="4">
+      <c r="N74" s="4">
         <v>3.54</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>363</v>
       </c>
@@ -9619,26 +10164,30 @@
       <c r="G75" s="2">
         <v>2</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H75" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I75" s="1" t="s">
+      <c r="J75" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="K75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="L75" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="L75" s="2">
+      <c r="M75" s="2">
         <v>0.27</v>
       </c>
-      <c r="M75" s="4">
+      <c r="N75" s="4">
         <v>0.54</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>364</v>
       </c>
@@ -9661,26 +10210,30 @@
       <c r="G76" s="2">
         <v>2</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="H76" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I76" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J76" s="1" t="s">
+      <c r="K76" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="L76" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="L76" s="2">
+      <c r="M76" s="2">
         <v>0.83</v>
       </c>
-      <c r="M76" s="4">
+      <c r="N76" s="4">
         <v>1.66</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>365</v>
       </c>
@@ -9703,26 +10256,30 @@
       <c r="G77" s="2">
         <v>2</v>
       </c>
-      <c r="H77" s="1" t="s">
+      <c r="H77" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I77" s="1" t="s">
+      <c r="J77" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J77" s="1" t="s">
+      <c r="K77" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K77" s="1" t="s">
+      <c r="L77" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="L77" s="2">
+      <c r="M77" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="M77" s="4">
+      <c r="N77" s="4">
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>366</v>
       </c>
@@ -9745,41 +10302,46 @@
       <c r="G78" s="9">
         <v>2</v>
       </c>
-      <c r="H78" s="8" t="s">
+      <c r="H78" s="2">
+        <f>RAW[[#This Row],[Quantity]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="I78" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="I78" s="8" t="s">
+      <c r="J78" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="J78" s="8" t="s">
+      <c r="K78" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K78" s="8" t="s">
+      <c r="L78" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="L78" s="9">
+      <c r="M78" s="9">
         <v>0.24</v>
       </c>
-      <c r="M78" s="10">
+      <c r="N78" s="10">
         <v>0.48</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="K1:K1048576 I1:I1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="L1:L1048576 J1:J1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{3C94E912-81AB-435E-AE90-6C5DA5196F58}">
-            <xm:f>COUNTIF('COMBINED PT2'!$H:$H,I2)&gt;0</xm:f>
+            <xm:f>COUNTIF('COMBINED PT2'!$H:$H,J2)&gt;0</xm:f>
             <x14:dxf>
               <font>
                 <b/>
@@ -9787,7 +10349,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I2:I78</xm:sqref>
+          <xm:sqref>J2:J78</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>